<commit_message>
bo xung comment va yeu cau goc
</commit_message>
<xml_diff>
--- a/DOCUMENT/DMS.xlsx
+++ b/DOCUMENT/DMS.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dungnt\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\DMS_PSHN\DOCUMENT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B3AE013-5BAC-4354-A274-9507232344D4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F376DAD1-F61A-4166-AC9B-8B85CD00D75A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{2BBEDB36-3A34-4925-BB5B-B63EA3348209}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{2BBEDB36-3A34-4925-BB5B-B63EA3348209}"/>
   </bookViews>
   <sheets>
     <sheet name="Đối tượng" sheetId="1" r:id="rId1"/>
@@ -1685,20 +1685,20 @@
   </sheetPr>
   <dimension ref="A1:G148"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="41.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="46.88671875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="32.5546875" customWidth="1"/>
-    <col min="5" max="5" width="46.33203125" style="9" customWidth="1"/>
-    <col min="6" max="6" width="57.33203125" style="10" customWidth="1"/>
+    <col min="2" max="2" width="41.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="32.5703125" customWidth="1"/>
+    <col min="5" max="5" width="46.28515625" style="9" customWidth="1"/>
+    <col min="6" max="6" width="57.28515625" style="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>371</v>
       </c>
@@ -1709,7 +1709,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="11" customFormat="1" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" s="11" customFormat="1" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>203</v>
       </c>
@@ -1725,7 +1725,7 @@
       <c r="E2" s="12"/>
       <c r="F2" s="17"/>
     </row>
-    <row r="3" spans="1:6" s="13" customFormat="1" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" s="13" customFormat="1" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="14"/>
       <c r="D3" s="13" t="s">
         <v>14</v>
@@ -1737,7 +1737,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.2" collapsed="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="26.25" collapsed="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1752,7 +1752,7 @@
       </c>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B5" s="2"/>
       <c r="C5" s="8"/>
       <c r="D5" s="3" t="s">
@@ -1762,7 +1762,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B6" s="2"/>
       <c r="C6" s="8"/>
       <c r="D6" s="3" t="s">
@@ -1772,7 +1772,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B7" s="2"/>
       <c r="C7" s="8"/>
       <c r="D7" s="4" t="s">
@@ -1782,7 +1782,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B8" s="5"/>
       <c r="C8" s="8"/>
       <c r="D8" s="6" t="s">
@@ -1792,7 +1792,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>
       <c r="C9" s="8"/>
       <c r="D9" s="6" t="s">
@@ -1802,7 +1802,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B10" s="2"/>
       <c r="C10" s="8"/>
       <c r="D10" s="6" t="s">
@@ -1812,7 +1812,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B11" s="7"/>
       <c r="C11" s="8"/>
       <c r="D11" s="3" t="s">
@@ -1822,7 +1822,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="3" t="s">
@@ -1832,7 +1832,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="55.2" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1850,7 +1850,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B14" s="2"/>
       <c r="C14" s="8"/>
       <c r="D14" s="3" t="s">
@@ -1858,7 +1858,7 @@
       </c>
       <c r="E14" s="8"/>
     </row>
-    <row r="15" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B15" s="2"/>
       <c r="C15" s="8"/>
       <c r="D15" s="3" t="s">
@@ -1868,7 +1868,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B16" s="2"/>
       <c r="C16" s="8"/>
       <c r="D16" s="3" t="s">
@@ -1878,7 +1878,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
       <c r="C17" s="8"/>
       <c r="D17" s="3" t="s">
@@ -1888,7 +1888,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B18" s="2"/>
       <c r="C18" s="8"/>
       <c r="D18" s="3" t="s">
@@ -1898,7 +1898,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B19" s="2"/>
       <c r="C19" s="8"/>
       <c r="D19" s="3" t="s">
@@ -1908,7 +1908,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B20" s="2"/>
       <c r="C20" s="8"/>
       <c r="D20" s="3" t="s">
@@ -1918,7 +1918,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B21" s="2"/>
       <c r="C21" s="8"/>
       <c r="D21" s="3" t="s">
@@ -1928,7 +1928,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B22" s="2"/>
       <c r="C22" s="8"/>
       <c r="D22" s="3" t="s">
@@ -1938,7 +1938,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" ht="12.75" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B23" s="2"/>
       <c r="C23" s="8"/>
       <c r="D23" s="16" t="s">
@@ -1948,7 +1948,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="13.8" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="12.75" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -1963,7 +1963,7 @@
       </c>
       <c r="E24" s="8"/>
     </row>
-    <row r="25" spans="1:5" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B25" s="2"/>
       <c r="C25" s="8"/>
       <c r="D25" s="3" t="s">
@@ -1971,7 +1971,7 @@
       </c>
       <c r="E25" s="8"/>
     </row>
-    <row r="26" spans="1:5" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B26" s="2"/>
       <c r="C26" s="8"/>
       <c r="D26" s="3" t="s">
@@ -1979,7 +1979,7 @@
       </c>
       <c r="E26" s="8"/>
     </row>
-    <row r="27" spans="1:5" ht="13.8" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="12.75" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4</v>
       </c>
@@ -1992,7 +1992,7 @@
       <c r="D27" s="3"/>
       <c r="E27" s="8"/>
     </row>
-    <row r="28" spans="1:5" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>5</v>
       </c>
@@ -2003,7 +2003,7 @@
       </c>
       <c r="E28" s="8"/>
     </row>
-    <row r="29" spans="1:5" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B29" s="2"/>
       <c r="C29" s="8"/>
       <c r="D29" s="3" t="s">
@@ -2011,7 +2011,7 @@
       </c>
       <c r="E29" s="8"/>
     </row>
-    <row r="30" spans="1:5" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B30" s="2"/>
       <c r="C30" s="8"/>
       <c r="D30" s="3" t="s">
@@ -2019,7 +2019,7 @@
       </c>
       <c r="E30" s="8"/>
     </row>
-    <row r="31" spans="1:5" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>6</v>
       </c>
@@ -2030,7 +2030,7 @@
       </c>
       <c r="E31" s="8"/>
     </row>
-    <row r="32" spans="1:5" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>7</v>
       </c>
@@ -2041,7 +2041,7 @@
       </c>
       <c r="E32" s="8"/>
     </row>
-    <row r="33" spans="1:6" ht="27.6" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" ht="25.5" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>5</v>
       </c>
@@ -2059,7 +2059,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="13.8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" ht="12.75" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="B34" s="2"/>
       <c r="C34" s="8"/>
       <c r="D34" s="3" t="s">
@@ -2067,7 +2067,7 @@
       </c>
       <c r="E34" s="8"/>
     </row>
-    <row r="35" spans="1:6" ht="13.8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" ht="12.75" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>8</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="13.8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" ht="12.75" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>9</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="13.8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="12.75" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="B37" s="2"/>
       <c r="C37" s="8"/>
       <c r="D37" s="3" t="s">
@@ -2103,7 +2103,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="38" spans="1:6" ht="13.8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" ht="12.75" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="B38" s="2"/>
       <c r="C38" s="8"/>
       <c r="D38" s="3" t="s">
@@ -2113,7 +2113,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="13.8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" ht="12.75" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>10</v>
       </c>
@@ -2126,7 +2126,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="13.8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" ht="12.75" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>11</v>
       </c>
@@ -2139,7 +2139,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="41" spans="1:6" ht="13.8" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" ht="12.75" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>6</v>
       </c>
@@ -2152,7 +2152,7 @@
       </c>
       <c r="E41" s="8"/>
     </row>
-    <row r="42" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B42" s="2"/>
       <c r="C42" s="8"/>
       <c r="D42" s="3" t="s">
@@ -2160,7 +2160,7 @@
       </c>
       <c r="E42" s="8"/>
     </row>
-    <row r="43" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>12</v>
       </c>
@@ -2173,7 +2173,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="44" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>13</v>
       </c>
@@ -2186,7 +2186,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B45" s="2"/>
       <c r="C45" s="8"/>
       <c r="D45" s="3" t="s">
@@ -2196,7 +2196,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B46" s="2"/>
       <c r="C46" s="8"/>
       <c r="D46" s="3" t="s">
@@ -2206,7 +2206,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>14</v>
       </c>
@@ -2219,7 +2219,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>15</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="69" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" ht="63.75" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>7</v>
       </c>
@@ -2247,7 +2247,7 @@
       </c>
       <c r="E49" s="8"/>
     </row>
-    <row r="50" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B50" s="2"/>
       <c r="C50" s="8"/>
       <c r="D50" s="3" t="s">
@@ -2255,7 +2255,7 @@
       </c>
       <c r="E50" s="8"/>
     </row>
-    <row r="51" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B51" s="2"/>
       <c r="C51" s="8"/>
       <c r="D51" s="3" t="s">
@@ -2263,7 +2263,7 @@
       </c>
       <c r="E51" s="8"/>
     </row>
-    <row r="52" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B52" s="2"/>
       <c r="C52" s="8"/>
       <c r="D52" s="3" t="s">
@@ -2271,7 +2271,7 @@
       </c>
       <c r="E52" s="8"/>
     </row>
-    <row r="53" spans="1:7" ht="41.4" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" ht="38.25" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>8</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B54" s="2"/>
       <c r="C54" s="8"/>
       <c r="D54" s="3" t="s">
@@ -2297,7 +2297,7 @@
       </c>
       <c r="E54" s="8"/>
     </row>
-    <row r="55" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B55" s="2"/>
       <c r="C55" s="8"/>
       <c r="D55" s="3" t="s">
@@ -2307,7 +2307,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B56" s="2"/>
       <c r="C56" s="8"/>
       <c r="D56" s="3" t="s">
@@ -2317,7 +2317,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B57" s="2"/>
       <c r="C57" s="8"/>
       <c r="D57" s="3" t="s">
@@ -2327,7 +2327,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B58" s="2"/>
       <c r="C58" s="8"/>
       <c r="D58" s="3" t="s">
@@ -2337,7 +2337,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B59" s="2"/>
       <c r="C59" s="8"/>
       <c r="D59" s="3" t="s">
@@ -2347,7 +2347,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B60" s="2"/>
       <c r="C60" s="8"/>
       <c r="D60" s="3" t="s">
@@ -2357,7 +2357,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="61" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B61" s="2"/>
       <c r="C61" s="8"/>
       <c r="D61" s="3" t="s">
@@ -2367,7 +2367,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B62" s="2"/>
       <c r="C62" s="8"/>
       <c r="D62" s="3" t="s">
@@ -2377,7 +2377,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="13.8" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" ht="12.75" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>9</v>
       </c>
@@ -2393,7 +2393,7 @@
       <c r="E63" s="8"/>
       <c r="G63" s="10"/>
     </row>
-    <row r="64" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B64" s="2"/>
       <c r="C64" s="8"/>
       <c r="D64" s="3" t="s">
@@ -2402,7 +2402,7 @@
       <c r="E64" s="8"/>
       <c r="G64" s="10"/>
     </row>
-    <row r="65" spans="1:7" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" ht="29.25" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B65" s="2"/>
       <c r="C65" s="8"/>
       <c r="D65" s="3" t="s">
@@ -2413,7 +2413,7 @@
       </c>
       <c r="G65" s="10"/>
     </row>
-    <row r="66" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B66" s="2"/>
       <c r="C66" s="8"/>
       <c r="D66" s="3" t="s">
@@ -2424,7 +2424,7 @@
       </c>
       <c r="G66" s="10"/>
     </row>
-    <row r="67" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B67" s="2"/>
       <c r="C67" s="8"/>
       <c r="D67" s="3" t="s">
@@ -2435,7 +2435,7 @@
       </c>
       <c r="G67" s="10"/>
     </row>
-    <row r="68" spans="1:7" ht="27.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" ht="25.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B68" s="2"/>
       <c r="C68" s="8"/>
       <c r="D68" s="3" t="s">
@@ -2446,7 +2446,7 @@
       </c>
       <c r="G68" s="10"/>
     </row>
-    <row r="69" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" ht="25.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B69" s="2"/>
       <c r="C69" s="8"/>
       <c r="D69" s="3" t="s">
@@ -2457,7 +2457,7 @@
       </c>
       <c r="G69" s="10"/>
     </row>
-    <row r="70" spans="1:7" ht="41.4" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" ht="38.25" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>10</v>
       </c>
@@ -2473,7 +2473,7 @@
       <c r="E70" s="8"/>
       <c r="G70" s="10"/>
     </row>
-    <row r="71" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B71" s="2"/>
       <c r="C71" s="8"/>
       <c r="D71" s="3" t="s">
@@ -2482,7 +2482,7 @@
       <c r="E71" s="8"/>
       <c r="G71" s="10"/>
     </row>
-    <row r="72" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B72" s="2"/>
       <c r="C72" s="8"/>
       <c r="D72" s="3" t="s">
@@ -2494,7 +2494,7 @@
       </c>
       <c r="G72" s="10"/>
     </row>
-    <row r="73" spans="1:7" ht="27.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" ht="25.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B73" s="2"/>
       <c r="C73" s="8"/>
       <c r="D73" s="3" t="s">
@@ -2508,7 +2508,7 @@
       </c>
       <c r="G73" s="10"/>
     </row>
-    <row r="74" spans="1:7" ht="13.8" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" ht="12.75" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>11</v>
       </c>
@@ -2524,7 +2524,7 @@
       <c r="E74" s="8"/>
       <c r="G74" s="10"/>
     </row>
-    <row r="75" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B75" s="2"/>
       <c r="C75" s="8"/>
       <c r="D75" s="3" t="s">
@@ -2533,7 +2533,7 @@
       <c r="E75" s="8"/>
       <c r="G75" s="10"/>
     </row>
-    <row r="76" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B76" s="2"/>
       <c r="C76" s="8"/>
       <c r="D76" s="3" t="s">
@@ -2544,7 +2544,7 @@
       </c>
       <c r="G76" s="10"/>
     </row>
-    <row r="77" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B77" s="2"/>
       <c r="C77" s="8"/>
       <c r="D77" s="3" t="s">
@@ -2555,7 +2555,7 @@
       </c>
       <c r="G77" s="10"/>
     </row>
-    <row r="78" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B78" s="2"/>
       <c r="C78" s="8"/>
       <c r="D78" s="3" t="s">
@@ -2566,7 +2566,7 @@
       </c>
       <c r="G78" s="10"/>
     </row>
-    <row r="79" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B79" s="2"/>
       <c r="C79" s="8"/>
       <c r="D79" s="3" t="s">
@@ -2577,7 +2577,7 @@
       </c>
       <c r="G79" s="10"/>
     </row>
-    <row r="80" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B80" s="2"/>
       <c r="C80" s="8"/>
       <c r="D80" s="3" t="s">
@@ -2588,7 +2588,7 @@
       </c>
       <c r="G80" s="10"/>
     </row>
-    <row r="81" spans="2:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B81" s="2"/>
       <c r="C81" s="8"/>
       <c r="D81" s="3" t="s">
@@ -2599,7 +2599,7 @@
       </c>
       <c r="G81" s="10"/>
     </row>
-    <row r="82" spans="2:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B82" s="2"/>
       <c r="C82" s="8"/>
       <c r="D82" s="3" t="s">
@@ -2610,7 +2610,7 @@
       </c>
       <c r="G82" s="10"/>
     </row>
-    <row r="83" spans="2:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B83" s="2"/>
       <c r="C83" s="8"/>
       <c r="D83" s="3" t="s">
@@ -2621,7 +2621,7 @@
       </c>
       <c r="G83" s="10"/>
     </row>
-    <row r="84" spans="2:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B84" s="2"/>
       <c r="C84" s="8"/>
       <c r="D84" s="3" t="s">
@@ -2632,7 +2632,7 @@
       </c>
       <c r="G84" s="10"/>
     </row>
-    <row r="85" spans="2:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B85" s="2"/>
       <c r="C85" s="8"/>
       <c r="D85" s="3" t="s">
@@ -2643,7 +2643,7 @@
       </c>
       <c r="G85" s="10"/>
     </row>
-    <row r="86" spans="2:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B86" s="2"/>
       <c r="C86" s="8"/>
       <c r="D86" s="3" t="s">
@@ -2654,7 +2654,7 @@
       </c>
       <c r="G86" s="10"/>
     </row>
-    <row r="87" spans="2:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B87" s="2"/>
       <c r="C87" s="8"/>
       <c r="D87" s="3" t="s">
@@ -2665,7 +2665,7 @@
       </c>
       <c r="G87" s="10"/>
     </row>
-    <row r="88" spans="2:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B88" s="2"/>
       <c r="C88" s="8"/>
       <c r="D88" s="3" t="s">
@@ -2676,7 +2676,7 @@
       </c>
       <c r="G88" s="10"/>
     </row>
-    <row r="89" spans="2:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B89" s="2"/>
       <c r="C89" s="8"/>
       <c r="D89" s="3" t="s">
@@ -2687,7 +2687,7 @@
       </c>
       <c r="G89" s="10"/>
     </row>
-    <row r="90" spans="2:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B90" s="2"/>
       <c r="C90" s="8"/>
       <c r="D90" s="3" t="s">
@@ -2701,7 +2701,7 @@
       </c>
       <c r="G90" s="10"/>
     </row>
-    <row r="91" spans="2:7" ht="27.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:7" ht="25.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B91" s="2"/>
       <c r="C91" s="8"/>
       <c r="D91" s="2" t="s">
@@ -2712,7 +2712,7 @@
       </c>
       <c r="G91" s="10"/>
     </row>
-    <row r="92" spans="2:7" ht="13.8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:7" ht="12.75" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="B92" s="2"/>
       <c r="C92" s="8"/>
       <c r="D92" s="3" t="s">
@@ -2723,7 +2723,7 @@
       </c>
       <c r="G92" s="10"/>
     </row>
-    <row r="93" spans="2:7" ht="27.6" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:7" ht="25.5" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="B93" s="2"/>
       <c r="C93" s="8"/>
       <c r="D93" s="3" t="s">
@@ -2734,7 +2734,7 @@
       </c>
       <c r="G93" s="10"/>
     </row>
-    <row r="94" spans="2:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B94" s="2"/>
       <c r="C94" s="8"/>
       <c r="D94" s="3" t="s">
@@ -2745,7 +2745,7 @@
       </c>
       <c r="G94" s="10"/>
     </row>
-    <row r="95" spans="2:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B95" s="2"/>
       <c r="C95" s="8"/>
       <c r="D95" s="3" t="s">
@@ -2756,7 +2756,7 @@
       </c>
       <c r="G95" s="10"/>
     </row>
-    <row r="96" spans="2:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B96" s="2"/>
       <c r="C96" s="8"/>
       <c r="D96" s="16" t="s">
@@ -2767,7 +2767,7 @@
       </c>
       <c r="G96" s="10"/>
     </row>
-    <row r="97" spans="1:7" ht="27.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" ht="25.5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B97" s="2"/>
       <c r="C97" s="8"/>
       <c r="D97" s="16" t="s">
@@ -2778,7 +2778,7 @@
       </c>
       <c r="G97" s="10"/>
     </row>
-    <row r="98" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B98" s="2"/>
       <c r="C98" s="8"/>
       <c r="D98" s="16" t="s">
@@ -2789,7 +2789,7 @@
       </c>
       <c r="G98" s="10"/>
     </row>
-    <row r="99" spans="1:7" ht="13.8" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" ht="12.75" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>12</v>
       </c>
@@ -2805,7 +2805,7 @@
       <c r="E99" s="8"/>
       <c r="G99" s="10"/>
     </row>
-    <row r="100" spans="1:7" ht="13.8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" ht="12.75" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="B100" s="2"/>
       <c r="C100" s="8"/>
       <c r="D100" s="3" t="s">
@@ -2814,7 +2814,7 @@
       <c r="E100" s="8"/>
       <c r="G100" s="10"/>
     </row>
-    <row r="101" spans="1:7" ht="13.8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" ht="12.75" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="B101" s="2"/>
       <c r="C101" s="8"/>
       <c r="D101" s="3" t="s">
@@ -2825,7 +2825,7 @@
       </c>
       <c r="G101" s="10"/>
     </row>
-    <row r="102" spans="1:7" ht="13.8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" ht="12.75" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="B102" s="2"/>
       <c r="C102" s="8"/>
       <c r="D102" s="3" t="s">
@@ -2836,7 +2836,7 @@
       </c>
       <c r="G102" s="10"/>
     </row>
-    <row r="103" spans="1:7" ht="13.8" hidden="1" outlineLevel="2" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" ht="12.75" hidden="1" outlineLevel="2" x14ac:dyDescent="0.2">
       <c r="B103" s="2"/>
       <c r="C103" s="8"/>
       <c r="D103" s="3" t="s">
@@ -2847,7 +2847,7 @@
       </c>
       <c r="G103" s="10"/>
     </row>
-    <row r="104" spans="1:7" ht="27.6" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" ht="25.5" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>13</v>
       </c>
@@ -2862,7 +2862,7 @@
       </c>
       <c r="E104" s="8"/>
     </row>
-    <row r="105" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B105" s="2"/>
       <c r="C105" s="8"/>
       <c r="D105" s="3" t="s">
@@ -2870,7 +2870,7 @@
       </c>
       <c r="E105" s="8"/>
     </row>
-    <row r="106" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B106" s="2"/>
       <c r="C106" s="8"/>
       <c r="D106" s="16" t="s">
@@ -2880,7 +2880,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="107" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B107" s="2"/>
       <c r="C107" s="8"/>
       <c r="D107" s="3" t="s">
@@ -2890,7 +2890,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="108" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B108" s="2"/>
       <c r="C108" s="8"/>
       <c r="D108" s="3" t="s">
@@ -2900,7 +2900,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B109" s="2"/>
       <c r="C109" s="8"/>
       <c r="D109" s="16" t="s">
@@ -2910,7 +2910,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="110" spans="1:7" ht="41.4" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" ht="38.25" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>14</v>
       </c>
@@ -2924,13 +2924,13 @@
         <v>170</v>
       </c>
     </row>
-    <row r="111" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B111" s="2"/>
       <c r="D111" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="112" spans="1:7" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B112" s="2"/>
       <c r="D112" t="s">
         <v>180</v>
@@ -2939,7 +2939,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="113" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B113" s="2"/>
       <c r="D113" t="s">
         <v>52</v>
@@ -2948,7 +2948,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="114" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B114" s="2"/>
       <c r="D114" t="s">
         <v>182</v>
@@ -2957,7 +2957,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="115" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B115" s="2"/>
       <c r="D115" t="s">
         <v>183</v>
@@ -2966,7 +2966,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="116" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B116" s="2"/>
       <c r="D116" t="s">
         <v>21</v>
@@ -2975,7 +2975,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="117" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B117" s="2"/>
       <c r="D117" t="s">
         <v>277</v>
@@ -2984,7 +2984,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="118" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B118" s="2"/>
       <c r="D118" t="s">
         <v>73</v>
@@ -2993,7 +2993,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="119" spans="1:6" ht="27.6" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:6" ht="25.5" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>15</v>
       </c>
@@ -3007,31 +3007,31 @@
         <v>171</v>
       </c>
     </row>
-    <row r="120" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B120" s="2"/>
       <c r="D120" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="121" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B121" s="2"/>
       <c r="D121" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="122" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B122" s="2"/>
       <c r="D122" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="123" spans="1:6" ht="13.8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:6" ht="12.75" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B123" s="2"/>
       <c r="D123" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="124" spans="1:6" ht="13.8" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:6" ht="12.75" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>16</v>
       </c>
@@ -3045,12 +3045,12 @@
         <v>165</v>
       </c>
     </row>
-    <row r="125" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D125" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="126" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D126" t="s">
         <v>55</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="127" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D127" t="s">
         <v>159</v>
       </c>
@@ -3066,7 +3066,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="128" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D128" t="s">
         <v>162</v>
       </c>
@@ -3074,7 +3074,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="13.8" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" ht="12.75" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>17</v>
       </c>
@@ -3085,12 +3085,12 @@
         <v>173</v>
       </c>
     </row>
-    <row r="130" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D130" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="131" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D131" t="s">
         <v>1</v>
       </c>
@@ -3098,7 +3098,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="132" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D132" t="s">
         <v>175</v>
       </c>
@@ -3106,7 +3106,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="133" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D133" t="s">
         <v>176</v>
       </c>
@@ -3114,7 +3114,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="134" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D134" t="s">
         <v>177</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="135" spans="1:5" ht="110.4" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" ht="102" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A135" s="25">
         <v>18</v>
       </c>
@@ -3133,12 +3133,12 @@
         <v>325</v>
       </c>
     </row>
-    <row r="136" spans="1:5" ht="13.8" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" ht="13.9" hidden="1" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C136" s="9" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="137" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C137" s="9" t="s">
         <v>1</v>
       </c>
@@ -3146,7 +3146,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="138" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C138" s="9" t="s">
         <v>73</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="139" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="C139" s="9" t="s">
         <v>93</v>
       </c>
@@ -3162,12 +3162,12 @@
         <v>313</v>
       </c>
     </row>
-    <row r="140" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D140" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="141" spans="1:5" ht="27.6" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" ht="26.25" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D141" t="s">
         <v>329</v>
       </c>
@@ -3175,7 +3175,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="142" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D142" t="s">
         <v>332</v>
       </c>
@@ -3183,7 +3183,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="143" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D143" t="s">
         <v>334</v>
       </c>
@@ -3191,7 +3191,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="144" spans="1:5" ht="55.2" collapsed="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" ht="51" collapsed="1" x14ac:dyDescent="0.2">
       <c r="A144" s="25">
         <v>19</v>
       </c>
@@ -3202,13 +3202,13 @@
         <v>324</v>
       </c>
     </row>
-    <row r="145" spans="4:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="4:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D145" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E145"/>
     </row>
-    <row r="146" spans="4:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="4:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D146" s="9" t="s">
         <v>327</v>
       </c>
@@ -3216,7 +3216,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="147" spans="4:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="4:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D147" t="s">
         <v>38</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="148" spans="4:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="4:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="D148" t="s">
         <v>334</v>
       </c>
@@ -3249,19 +3249,19 @@
       <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="9"/>
-    <col min="2" max="2" width="35.21875" style="9" customWidth="1"/>
-    <col min="3" max="3" width="25.88671875" style="9" customWidth="1"/>
-    <col min="4" max="4" width="36.5546875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="31.5546875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="23.21875" style="9" customWidth="1"/>
-    <col min="7" max="7" width="39.44140625" style="9" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="9"/>
+    <col min="1" max="1" width="8.85546875" style="9"/>
+    <col min="2" max="2" width="35.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="36.5703125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="31.5703125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" style="9" customWidth="1"/>
+    <col min="7" max="7" width="39.42578125" style="9" customWidth="1"/>
+    <col min="8" max="16384" width="8.85546875" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="19.899999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="26" t="s">
         <v>242</v>
       </c>
@@ -3270,7 +3270,7 @@
       <c r="D1" s="26"/>
       <c r="E1" s="26"/>
     </row>
-    <row r="2" spans="1:5" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="21" t="s">
         <v>203</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="30.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="30.6" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -3304,7 +3304,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A4" s="9">
         <v>2</v>
       </c>
@@ -3318,7 +3318,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <v>3</v>
       </c>
@@ -3332,7 +3332,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="20"/>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
@@ -3341,7 +3341,7 @@
       </c>
       <c r="E6" s="20"/>
     </row>
-    <row r="7" spans="1:5" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="21" t="s">
         <v>203</v>
       </c>
@@ -3356,7 +3356,7 @@
       </c>
       <c r="E7" s="21"/>
     </row>
-    <row r="8" spans="1:5" customFormat="1" ht="28.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" customFormat="1" ht="26.25" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -3370,7 +3370,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>2</v>
       </c>
@@ -3384,7 +3384,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
         <v>3</v>
       </c>
@@ -3398,7 +3398,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>4</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="26" t="s">
         <v>275</v>
       </c>
@@ -3421,7 +3421,7 @@
       <c r="D13" s="26"/>
       <c r="E13" s="26"/>
     </row>
-    <row r="14" spans="1:5" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="21" t="s">
         <v>203</v>
       </c>
@@ -3438,7 +3438,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9">
         <v>1</v>
       </c>
@@ -3449,7 +3449,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="9">
         <v>2</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="9">
         <v>3</v>
       </c>
@@ -3471,7 +3471,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="26" t="s">
         <v>274</v>
       </c>
@@ -3482,7 +3482,7 @@
       <c r="F19" s="26"/>
       <c r="G19" s="26"/>
     </row>
-    <row r="20" spans="1:7" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="21" t="s">
         <v>203</v>
       </c>
@@ -3505,7 +3505,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="50.4" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="50.45" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9">
         <v>1</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" s="9">
         <v>2</v>
       </c>
@@ -3542,7 +3542,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9">
         <v>3</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9">
         <v>4</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9">
         <v>5</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="46.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9">
         <v>6</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="35.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9">
         <v>7</v>
       </c>
@@ -3636,7 +3636,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="29.45" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9">
         <v>8</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9">
         <v>9</v>
       </c>
@@ -3661,7 +3661,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A32" s="9">
         <v>10</v>
       </c>
@@ -3681,7 +3681,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A33" s="9">
         <v>11</v>
       </c>
@@ -3715,22 +3715,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74CBB556-8F07-4551-8AF5-26DCAC65A6ED}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="46.33203125" style="9" customWidth="1"/>
-    <col min="3" max="3" width="29.6640625" customWidth="1"/>
-    <col min="4" max="4" width="22.21875" customWidth="1"/>
-    <col min="5" max="5" width="16.5546875" customWidth="1"/>
-    <col min="6" max="7" width="19.21875" customWidth="1"/>
+    <col min="2" max="2" width="46.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="29.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="7" width="19.28515625" customWidth="1"/>
     <col min="8" max="8" width="29" customWidth="1"/>
-    <col min="9" max="9" width="21.77734375" customWidth="1"/>
+    <col min="9" max="9" width="21.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>369</v>
       </c>
@@ -3741,12 +3741,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
         <v>203</v>
       </c>
@@ -3775,7 +3775,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>3</v>
       </c>
@@ -3847,7 +3847,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>4</v>
       </c>
@@ -3876,7 +3876,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>5</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="69" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" ht="63.75" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>6</v>
       </c>
@@ -3934,7 +3934,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>7</v>
       </c>
@@ -3963,7 +3963,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
@@ -3992,7 +3992,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
@@ -4000,7 +4000,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>10</v>
       </c>
@@ -4008,7 +4008,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>11</v>
       </c>
@@ -4016,7 +4016,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>12</v>
       </c>
@@ -4024,7 +4024,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>13</v>
       </c>
@@ -4032,7 +4032,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>14</v>
       </c>
@@ -4040,7 +4040,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>15</v>
       </c>
@@ -4048,7 +4048,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>16</v>
       </c>
@@ -4056,7 +4056,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>17</v>
       </c>
@@ -4064,27 +4064,27 @@
         <v>338</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>22</v>
       </c>
@@ -4108,15 +4108,15 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="31.21875" customWidth="1"/>
-    <col min="3" max="3" width="35.77734375" customWidth="1"/>
-    <col min="4" max="4" width="62.88671875" customWidth="1"/>
-    <col min="5" max="5" width="39.77734375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
+    <col min="4" max="4" width="62.85546875" customWidth="1"/>
+    <col min="5" max="5" width="39.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>373</v>
       </c>
@@ -4127,7 +4127,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>203</v>
       </c>
@@ -4144,7 +4144,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4152,7 +4152,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4160,7 +4160,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4176,7 +4176,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4184,7 +4184,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4200,7 +4200,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4208,7 +4208,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -4216,7 +4216,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -4224,7 +4224,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -4232,7 +4232,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -4240,7 +4240,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -4256,7 +4256,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -4264,7 +4264,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -4272,7 +4272,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -4280,7 +4280,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -4288,7 +4288,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -4296,7 +4296,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -4304,7 +4304,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -4320,7 +4320,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -4328,7 +4328,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -4336,7 +4336,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -4344,7 +4344,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -4352,7 +4352,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -4360,7 +4360,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -4368,7 +4368,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -4392,13 +4392,13 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="22.5546875" customWidth="1"/>
-    <col min="3" max="3" width="39.6640625" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" customWidth="1"/>
+    <col min="3" max="3" width="39.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>370</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>203</v>
       </c>
@@ -4420,7 +4420,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="14.4" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -4431,7 +4431,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -4439,7 +4439,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -4447,7 +4447,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -4455,7 +4455,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -4466,7 +4466,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -4477,7 +4477,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -4488,7 +4488,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -4508,23 +4508,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97183150-1748-4C71-9404-9956C4121891}">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="68" customWidth="1"/>
-    <col min="4" max="4" width="37.33203125" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>203</v>
       </c>
@@ -4538,7 +4538,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="14.4" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:4" ht="13.5" thickTop="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>